<commit_message>
Better question in ex.2 on text manip.
</commit_message>
<xml_diff>
--- a/exercises/exercises02.xlsx
+++ b/exercises/exercises02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ad83bda99cce0ca/Github/ELE-3915/exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3691" documentId="8_{29B8196C-0F94-4E63-9C97-551F1F758BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54CAFD0C-00B8-4375-9C84-5E35F3CD0F98}"/>
+  <xr:revisionPtr revIDLastSave="3696" documentId="8_{29B8196C-0F94-4E63-9C97-551F1F758BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78E1B3FB-6AC7-4339-8600-FE85D74B8CBB}"/>
   <bookViews>
-    <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="965" firstSheet="1" activeTab="1" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="965" firstSheet="1" activeTab="4" xr2:uid="{58F8946E-589F-43AA-8127-245E86DA602D}"/>
   </bookViews>
   <sheets>
     <sheet name="Shirt sales" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="800">
   <si>
     <t>Male</t>
   </si>
@@ -2267,21 +2267,6 @@
   </si>
   <si>
     <t>You can’t connect the dots looking forward; you can only connect them looking backwards. So you have to trust that the dots will somehow connect in your future.</t>
-  </si>
-  <si>
-    <t>Write a formula that counts how many times the</t>
-  </si>
-  <si>
-    <t>word in the orange box appears in a text. Use the</t>
-  </si>
-  <si>
-    <t>formula to count the number of words in the</t>
-  </si>
-  <si>
-    <t>to see how I made a function counting the number of</t>
-  </si>
-  <si>
-    <t>words.)</t>
   </si>
   <si>
     <t>Exercise3</t>
@@ -2504,32 +2489,6 @@
     <t>Remember to use =&gt; and &lt;= for inequalities!</t>
   </si>
   <si>
-    <r>
-      <t>sentences of Table 2. (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Hint:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Look at the lecture notes</t>
-    </r>
-  </si>
-  <si>
     <t>You need to subsititute every instance of the word for</t>
   </si>
   <si>
@@ -2570,6 +2529,30 @@
   </si>
   <si>
     <t>b) What is the total sales of salespeople with first name ending in "e" with shirt size "S" or smaller?</t>
+  </si>
+  <si>
+    <t>Write a formula that counts how many times the word</t>
+  </si>
+  <si>
+    <t>in the orange box appears in a text. Use the formula to</t>
+  </si>
+  <si>
+    <t>count the number of words in the sentences of Table</t>
+  </si>
+  <si>
+    <t>2. The formula does not have to work for text starting</t>
+  </si>
+  <si>
+    <t>with the word ("Of course I love television!") or text</t>
+  </si>
+  <si>
+    <t>with adjacent instances of the word ("of of of") (Hint:</t>
+  </si>
+  <si>
+    <t>Look at the lecture notes to see how I made a function</t>
+  </si>
+  <si>
+    <t>counting the number of words.)</t>
   </si>
 </sst>
 </file>
@@ -2948,6 +2931,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="11"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2955,12 +2944,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10900,7 +10883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC0C6B7-48AE-4BCD-ADF0-20CF516D0AD5}">
   <dimension ref="A1:J214"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -10919,29 +10902,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>456</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="F2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>457</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -11078,7 +11061,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -11143,37 +11126,37 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>461</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="E27" s="25" t="s">
-        <v>747</v>
-      </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
+      <c r="E27" s="27" t="s">
+        <v>742</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -11195,7 +11178,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -11214,7 +11197,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -11233,7 +11216,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -11252,7 +11235,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -11271,7 +11254,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -11290,7 +11273,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -11309,7 +11292,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -11371,41 +11354,41 @@
       <c r="I40" s="9"/>
     </row>
     <row r="116" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
-      <c r="G116" s="28"/>
-      <c r="H116" s="28"/>
-      <c r="I116" s="28"/>
-      <c r="J116" s="28"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="25"/>
+      <c r="H116" s="25"/>
+      <c r="I116" s="25"/>
+      <c r="J116" s="25"/>
     </row>
     <row r="117" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
-      <c r="E118" s="25" t="s">
-        <v>748</v>
-      </c>
-      <c r="F118" s="25"/>
-      <c r="G118" s="25"/>
-      <c r="H118" s="25"/>
+      <c r="E118" s="27" t="s">
+        <v>743</v>
+      </c>
+      <c r="F118" s="27"/>
+      <c r="G118" s="27"/>
+      <c r="H118" s="27"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="E119" s="12" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>436</v>
@@ -11414,12 +11397,12 @@
         <v>437</v>
       </c>
       <c r="H119" s="12" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -11435,7 +11418,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -11451,7 +11434,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -11467,7 +11450,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -11483,7 +11466,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -11543,7 +11526,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E130" s="22" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -11552,18 +11535,18 @@
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E132" s="24" t="s">
-        <v>735</v>
-      </c>
-      <c r="F132" s="24"/>
-      <c r="G132" s="24"/>
+      <c r="E132" s="26" t="s">
+        <v>730</v>
+      </c>
+      <c r="F132" s="26"/>
+      <c r="G132" s="26"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E133" s="22" t="s">
         <v>439</v>
       </c>
       <c r="G133" s="22" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -11575,18 +11558,18 @@
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E135" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="F135" s="24"/>
-      <c r="G135" s="24"/>
+      <c r="E135" s="26" t="s">
+        <v>729</v>
+      </c>
+      <c r="F135" s="26"/>
+      <c r="G135" s="26"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E136" s="22" t="s">
         <v>439</v>
       </c>
       <c r="G136" s="22" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
@@ -11598,27 +11581,27 @@
       </c>
     </row>
     <row r="140" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="28" t="s">
+      <c r="A140" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="B140" s="28"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="28"/>
-      <c r="E140" s="28"/>
-      <c r="F140" s="28"/>
-      <c r="G140" s="28"/>
-      <c r="H140" s="28"/>
-      <c r="I140" s="28"/>
-      <c r="J140" s="28"/>
+      <c r="B140" s="25"/>
+      <c r="C140" s="25"/>
+      <c r="D140" s="25"/>
+      <c r="E140" s="25"/>
+      <c r="F140" s="25"/>
+      <c r="G140" s="25"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="25"/>
     </row>
     <row r="141" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="142" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E142" s="26" t="s">
-        <v>739</v>
-      </c>
-      <c r="F142" s="26"/>
-      <c r="G142" s="26"/>
-      <c r="H142" s="26"/>
+      <c r="E142" s="28" t="s">
+        <v>734</v>
+      </c>
+      <c r="F142" s="28"/>
+      <c r="G142" s="28"/>
+      <c r="H142" s="28"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E143" s="12" t="s">
@@ -12583,6 +12566,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E142:H142"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A1:J1"/>
@@ -12593,7 +12577,6 @@
     <mergeCell ref="E135:G135"/>
     <mergeCell ref="E118:H118"/>
     <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E142:H142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -12619,27 +12602,27 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
@@ -12765,16 +12748,16 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>461</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12813,12 +12796,12 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -12828,15 +12811,15 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="B22" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="B23" t="s">
         <v>471</v>
@@ -12844,20 +12827,20 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12872,16 +12855,16 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12896,16 +12879,16 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="25" t="s">
         <v>474</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12973,7 +12956,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -13196,7 +13179,7 @@
         <v>275.74</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -13239,7 +13222,7 @@
         <v>619.99</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -13282,7 +13265,7 @@
         <v>820.11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -13325,7 +13308,7 @@
         <v>530.17999999999995</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -13368,7 +13351,7 @@
         <v>288.2</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -13431,7 +13414,7 @@
         <v>756.29</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -13474,7 +13457,7 @@
         <v>409.45</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -13517,7 +13500,7 @@
         <v>383.62</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -13560,7 +13543,7 @@
         <v>894.16</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -13603,7 +13586,7 @@
         <v>215.38</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -13646,7 +13629,7 @@
         <v>679.21</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -17018,10 +17001,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3F554-9FA9-4B23-99A2-5E258CD0F3F7}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17034,26 +17017,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>456</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -17163,19 +17146,19 @@
       <c r="C16" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="25" t="s">
         <v>461</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>719</v>
+        <v>792</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>711</v>
@@ -17186,26 +17169,26 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>720</v>
+        <v>793</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="C22" s="25" t="s">
+        <v>794</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>783</v>
+      <c r="A23" s="1" t="s">
+        <v>795</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>713</v>
@@ -17216,7 +17199,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>722</v>
+        <v>796</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -17227,7 +17210,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>723</v>
+        <v>797</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -17237,6 +17220,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>798</v>
+      </c>
       <c r="C26">
         <v>2</v>
       </c>
@@ -17245,146 +17231,153 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>784</v>
+      <c r="A27" s="1" t="s">
+        <v>799</v>
       </c>
       <c r="E27" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>785</v>
-      </c>
       <c r="E28" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
-        <v>724</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>747</v>
-      </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>750</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>751</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>480</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="C34" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="C35" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="s">
+        <v>719</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="C36" t="s">
-        <v>760</v>
-      </c>
+        <v>744</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>742</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="C37" t="s">
-        <v>761</v>
+        <v>747</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>746</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="C38" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="C39" t="s">
-        <v>763</v>
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>723</v>
+      </c>
       <c r="C40" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>788</v>
+      <c r="A41" s="1" t="s">
+        <v>724</v>
       </c>
       <c r="C41" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>789</v>
+      <c r="A42" s="1" t="s">
+        <v>725</v>
       </c>
       <c r="C42" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>790</v>
+      <c r="A43" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C43" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="C45" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="C46" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>784</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="C36:F36"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="C32:F32"/>
     <mergeCell ref="C22:F22"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>

</xml_diff>